<commit_message>
771399 Updated for T23
</commit_message>
<xml_diff>
--- a/Test/Build 8/TAS eBill Defect Log IB_2.0_623.xlsx
+++ b/Test/Build 8/TAS eBill Defect Log IB_2.0_623.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\eBilling Docs\Build 7&amp;8&amp;9\Docs\All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D89471-68B8-4D60-997F-D8259A00031C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA0D453-CF04-4CAB-A0AD-97CDD2E849AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10344" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="143">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -142,8 +142,308 @@
     </r>
   </si>
   <si>
+    <t>CIT-Populate "OldValue" Column when No Room for Claim Office ID US3994 ID</t>
+  </si>
+  <si>
+    <t>DE854</t>
+  </si>
+  <si>
+    <t>TC3416:  CIT-eBilling-TS2–SYS Displays Original Claim Office ID When One Exists–Prod Only_US3994</t>
+  </si>
+  <si>
+    <t>DE871</t>
+  </si>
+  <si>
+    <t>UAT - INS record for SNF -Unit of service</t>
+  </si>
+  <si>
+    <t>US9 - Transmitting SNF Claims with Appropriate Revenue (USEB-16)</t>
+  </si>
+  <si>
+    <t>CIT - Dental Mock up Item 24 not pulling correct date</t>
+  </si>
+  <si>
+    <t>DE883</t>
+  </si>
+  <si>
+    <t>US1108: Enter/Edit Dental Claims</t>
+  </si>
+  <si>
+    <t>CIT - Dental Mock up Item 29a is not pulling any data</t>
+  </si>
+  <si>
+    <t>DE884</t>
+  </si>
+  <si>
+    <t>US4055: Dental Claims Mock-up</t>
+  </si>
+  <si>
+    <t>TC3437: CIT - eBilling - Dental Claim Mock up US4055</t>
+  </si>
+  <si>
+    <t>CIT - Mock up Dental Item 35 no number</t>
+  </si>
+  <si>
+    <t>DE885</t>
+  </si>
+  <si>
+    <t>CIT - Rendering needes to be changed to Rendering or Assistant Surgeon</t>
+  </si>
+  <si>
+    <t>DE891</t>
+  </si>
+  <si>
+    <t>CIT-Alternate Payer ID Not Transmitting to Secondary Claim_US4100</t>
+  </si>
+  <si>
+    <t>DE892</t>
+  </si>
+  <si>
+    <t>US4100: Alternate Payer ID</t>
+  </si>
+  <si>
+    <t>TC3493:  CIT-eBilling-TS1-Alternate Inst Payer IDs-US4100</t>
+  </si>
+  <si>
+    <t>TC1250: CIT eBilling TS2 Manual Dental Claim – Claim Level(1) US1108 and US131</t>
+  </si>
+  <si>
+    <t>UAT: Add Legend to Report for No Room to Update Data</t>
+  </si>
+  <si>
+    <t>US3995: Payer ID Report-Secondary Payer ID</t>
+  </si>
+  <si>
+    <t>TC3419: CIT-eBilling-TC1-HCCH Payer ID Report–Claims Office IDs–Prod Only_US3995</t>
+  </si>
+  <si>
+    <t>DE896</t>
+  </si>
+  <si>
+    <t>DE907</t>
+  </si>
+  <si>
+    <t>CIT - Dental Claim Mock up   - Column 31 does not display the correct amount</t>
+  </si>
+  <si>
+    <t>CIT  - Columns are too close together</t>
+  </si>
+  <si>
+    <t>DE908</t>
+  </si>
+  <si>
+    <t>CIT - Dental Claim Mock up 29A and 34A</t>
+  </si>
+  <si>
+    <t>DE915</t>
+  </si>
+  <si>
+    <t>CIT - Dental Mock up the tooth information for print was not get reset between procedure lines</t>
+  </si>
+  <si>
+    <t>DE918</t>
+  </si>
+  <si>
+    <t>CIT - Inst Claim Alt Payer ID Not Populated to Sec Claim_US4100</t>
+  </si>
+  <si>
+    <t>DE920</t>
+  </si>
+  <si>
+    <t>TS3494: CIT-eBilling-TS2-Alternate Prof Payer IDs-US4100</t>
+  </si>
+  <si>
+    <t>CIT - Dental Mock up display change</t>
+  </si>
+  <si>
+    <t>DE934</t>
+  </si>
+  <si>
+    <t>CIT - Dental Mock up -  Col 29a</t>
+  </si>
+  <si>
+    <t>DE940</t>
+  </si>
+  <si>
+    <t>CIT - Dental Mock up - General help</t>
+  </si>
+  <si>
+    <t>DE941</t>
+  </si>
+  <si>
+    <t>CIT - Dental Mock up A is not displayed in 29a</t>
+  </si>
+  <si>
+    <t>DE944</t>
+  </si>
+  <si>
+    <t>CIT - ROI bill creates fatal system error when closing bill</t>
+  </si>
+  <si>
+    <t>DE1071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/10/2018 Found in IB*2.0*623_T1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/12/2018 Found in IB*2.0*623_T3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/19/2018 Found in IB*2.0*623_T5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/30/2018 Found in IB*2.0*623_T6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/31/2018 Found in IB*2.0*623_T6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/1/2018 Found in IB*2.0*623_T6 </t>
+  </si>
+  <si>
+    <t>8/6/2018 Found in IB*2.0*623_T7</t>
+  </si>
+  <si>
+    <t>8/7/2018 Found in IB*2.0*623_T7</t>
+  </si>
+  <si>
+    <t>8/15/2018 Found in IB*2.0*623_T8</t>
+  </si>
+  <si>
+    <t>8/20/2018 Found in IB*2.0*623_T8</t>
+  </si>
+  <si>
+    <t>9/10/2018 Found in IB*2.0*623_T11</t>
+  </si>
+  <si>
+    <t>9/13/2018 Found in IB*2.0*623_T12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/19/2018 Verified in IB*2.0*623_T14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/17/2018 Verified in IB*2.0*623_T2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/17/2018 Verified in IB*2.0*623_T4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/2/2018 Verified in IB*2.0*623_T7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/7/2018 Verified in IB*2.0*623_T8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/31/2018 Verified in IB*2.0*623_T9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/28/2018 Verified in IB*2.0*623_T9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/22/2018 Verified in IB*2.0*623_T9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/17/2018 Verified in IB*2.0*623_T13 </t>
+  </si>
+  <si>
+    <t>US4995 - Implement Release of Information</t>
+  </si>
+  <si>
+    <t>1/7/2019 Found in IB*2.0*623_T15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/11/2019 Verified in IB*2.0*623_T16 </t>
+  </si>
+  <si>
+    <t>DE1074</t>
+  </si>
+  <si>
+    <t>CIT-CSA Worklist MINIMUM # OF DAYS Not working</t>
+  </si>
+  <si>
+    <t>US141 - CSA_Separate TRICARE/CHAMPVA (USEB-43)</t>
+  </si>
+  <si>
+    <t>TC4102: CIT-eBilling-TS1- Generate CSA Worklists by Non-MCCF, MCCF or Both Rate Types_US141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/15/2019 Verified in IB*2.0*623_T16 </t>
+  </si>
+  <si>
+    <t>CIT - Final Bill screen is incorrect</t>
+  </si>
+  <si>
+    <t>DE1075</t>
+  </si>
+  <si>
+    <t>US3346 - [Continued] Transmit 837 Transactions Through New Platform</t>
+  </si>
+  <si>
+    <t>TC3405: CIT - eBilling - Transmit 837 Transactions Through New Platform - Outpatient UB04– US3346</t>
+  </si>
+  <si>
+    <t>1/14/2019 Found in IB*2.0*623_T16</t>
+  </si>
+  <si>
+    <t>CIT - system is unable to id the correct Batch number if in a queue for FHIR and the switch is set to off</t>
+  </si>
+  <si>
+    <t>DE1076</t>
+  </si>
+  <si>
+    <t>1/16/2019 Found in IB*2.0*623_T16</t>
+  </si>
+  <si>
+    <t>TC3967 - CIT - eBilling Implement Release of Information – Outpatient 1500 Professional Claim_US4995 and TC3968: CIT-eBilling Implement Release of Information – Outpatient UB04 Institutional Claim</t>
+  </si>
+  <si>
+    <t>7/31/2018 Found in IB*2.0*623_T7</t>
+  </si>
+  <si>
+    <t>8/7/2018 Verified in IB*2.0*623_T8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/22/2019 Verified in IB*2.0*623_T20 </t>
+  </si>
+  <si>
+    <t>UAT defect</t>
+  </si>
+  <si>
+    <t>May 2019</t>
+  </si>
+  <si>
+    <t>DE1305</t>
+  </si>
+  <si>
+    <t>CIT- eBilling -Imprecise dates in claims</t>
+  </si>
+  <si>
+    <t>4/11/2019 Found in IB*2.0*623 T20</t>
+  </si>
+  <si>
+    <t>6/20/2019 Verified in IB*2.0*623 T22</t>
+  </si>
+  <si>
+    <t>IOC -  IB*2.0*623 v21 IOC Patch Tracking Message</t>
+  </si>
+  <si>
+    <t>DE1440</t>
+  </si>
+  <si>
+    <t>5/28/2019 Found in IB*2.0*623 T21</t>
+  </si>
+  <si>
+    <t>IOC - RPC Packaging Error</t>
+  </si>
+  <si>
+    <t>DE1441</t>
+  </si>
+  <si>
+    <t>July 2019</t>
+  </si>
+  <si>
     <r>
-      <t>Version 1.0</t>
+      <t>Version 2.0</t>
     </r>
     <r>
       <rPr>
@@ -157,274 +457,46 @@
     </r>
   </si>
   <si>
-    <t>CIT-Populate "OldValue" Column when No Room for Claim Office ID US3994 ID</t>
-  </si>
-  <si>
-    <t>DE854</t>
-  </si>
-  <si>
-    <t>TC3416:  CIT-eBilling-TS2–SYS Displays Original Claim Office ID When One Exists–Prod Only_US3994</t>
-  </si>
-  <si>
-    <t>DE871</t>
-  </si>
-  <si>
-    <t>UAT - INS record for SNF -Unit of service</t>
-  </si>
-  <si>
-    <t>US9 - Transmitting SNF Claims with Appropriate Revenue (USEB-16)</t>
-  </si>
-  <si>
-    <t>CIT - Dental Mock up Item 24 not pulling correct date</t>
-  </si>
-  <si>
-    <t>DE883</t>
-  </si>
-  <si>
-    <t>US1108: Enter/Edit Dental Claims</t>
-  </si>
-  <si>
-    <t>CIT - Dental Mock up Item 29a is not pulling any data</t>
-  </si>
-  <si>
-    <t>DE884</t>
-  </si>
-  <si>
-    <t>US4055: Dental Claims Mock-up</t>
-  </si>
-  <si>
-    <t>TC3437: CIT - eBilling - Dental Claim Mock up US4055</t>
-  </si>
-  <si>
-    <t>CIT - Mock up Dental Item 35 no number</t>
-  </si>
-  <si>
-    <t>DE885</t>
-  </si>
-  <si>
-    <t>CIT - Rendering needes to be changed to Rendering or Assistant Surgeon</t>
-  </si>
-  <si>
-    <t>DE891</t>
-  </si>
-  <si>
-    <t>CIT-Alternate Payer ID Not Transmitting to Secondary Claim_US4100</t>
-  </si>
-  <si>
-    <t>DE892</t>
-  </si>
-  <si>
-    <t>US4100: Alternate Payer ID</t>
-  </si>
-  <si>
-    <t>TC3493:  CIT-eBilling-TS1-Alternate Inst Payer IDs-US4100</t>
-  </si>
-  <si>
-    <t>TC1250: CIT eBilling TS2 Manual Dental Claim – Claim Level(1) US1108 and US131</t>
-  </si>
-  <si>
-    <t>UAT: Add Legend to Report for No Room to Update Data</t>
-  </si>
-  <si>
-    <t>US3995: Payer ID Report-Secondary Payer ID</t>
-  </si>
-  <si>
-    <t>TC3419: CIT-eBilling-TC1-HCCH Payer ID Report–Claims Office IDs–Prod Only_US3995</t>
-  </si>
-  <si>
-    <t>DE896</t>
-  </si>
-  <si>
-    <t>DE907</t>
-  </si>
-  <si>
-    <t>CIT - Dental Claim Mock up   - Column 31 does not display the correct amount</t>
-  </si>
-  <si>
-    <t>CIT  - Columns are too close together</t>
-  </si>
-  <si>
-    <t>DE908</t>
-  </si>
-  <si>
-    <t>CIT - Dental Claim Mock up 29A and 34A</t>
-  </si>
-  <si>
-    <t>DE915</t>
-  </si>
-  <si>
-    <t>CIT - Dental Mock up the tooth information for print was not get reset between procedure lines</t>
-  </si>
-  <si>
-    <t>DE918</t>
-  </si>
-  <si>
-    <t>CIT - Inst Claim Alt Payer ID Not Populated to Sec Claim_US4100</t>
-  </si>
-  <si>
-    <t>DE920</t>
-  </si>
-  <si>
-    <t>TS3494: CIT-eBilling-TS2-Alternate Prof Payer IDs-US4100</t>
-  </si>
-  <si>
-    <t>CIT - Dental Mock up display change</t>
-  </si>
-  <si>
-    <t>DE934</t>
-  </si>
-  <si>
-    <t>CIT - Dental Mock up -  Col 29a</t>
-  </si>
-  <si>
-    <t>DE940</t>
-  </si>
-  <si>
-    <t>CIT - Dental Mock up - General help</t>
-  </si>
-  <si>
-    <t>DE941</t>
-  </si>
-  <si>
-    <t>CIT - Dental Mock up A is not displayed in 29a</t>
-  </si>
-  <si>
-    <t>DE944</t>
-  </si>
-  <si>
-    <t>CIT - ROI bill creates fatal system error when closing bill</t>
-  </si>
-  <si>
-    <t>DE1071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/10/2018 Found in IB*2.0*623_T1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/12/2018 Found in IB*2.0*623_T3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/19/2018 Found in IB*2.0*623_T5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/30/2018 Found in IB*2.0*623_T6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/31/2018 Found in IB*2.0*623_T6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/1/2018 Found in IB*2.0*623_T6 </t>
-  </si>
-  <si>
-    <t>8/6/2018 Found in IB*2.0*623_T7</t>
-  </si>
-  <si>
-    <t>8/7/2018 Found in IB*2.0*623_T7</t>
-  </si>
-  <si>
-    <t>8/15/2018 Found in IB*2.0*623_T8</t>
-  </si>
-  <si>
-    <t>8/20/2018 Found in IB*2.0*623_T8</t>
-  </si>
-  <si>
-    <t>9/10/2018 Found in IB*2.0*623_T11</t>
-  </si>
-  <si>
-    <t>9/13/2018 Found in IB*2.0*623_T12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9/19/2018 Verified in IB*2.0*623_T14 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/17/2018 Verified in IB*2.0*623_T2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/17/2018 Verified in IB*2.0*623_T4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/2/2018 Verified in IB*2.0*623_T7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/7/2018 Verified in IB*2.0*623_T8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/31/2018 Verified in IB*2.0*623_T9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/28/2018 Verified in IB*2.0*623_T9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/22/2018 Verified in IB*2.0*623_T9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">9/17/2018 Verified in IB*2.0*623_T13 </t>
-  </si>
-  <si>
-    <t>US4995 - Implement Release of Information</t>
-  </si>
-  <si>
-    <t>1/7/2019 Found in IB*2.0*623_T15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/11/2019 Verified in IB*2.0*623_T16 </t>
-  </si>
-  <si>
-    <t>DE1074</t>
-  </si>
-  <si>
-    <t>CIT-CSA Worklist MINIMUM # OF DAYS Not working</t>
-  </si>
-  <si>
-    <t>US141 - CSA_Separate TRICARE/CHAMPVA (USEB-43)</t>
-  </si>
-  <si>
-    <t>TC4102: CIT-eBilling-TS1- Generate CSA Worklists by Non-MCCF, MCCF or Both Rate Types_US141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/15/2019 Verified in IB*2.0*623_T16 </t>
-  </si>
-  <si>
-    <t>CIT - Final Bill screen is incorrect</t>
-  </si>
-  <si>
-    <t>DE1075</t>
-  </si>
-  <si>
-    <t>US3346 - [Continued] Transmit 837 Transactions Through New Platform</t>
-  </si>
-  <si>
-    <t>TC3405: CIT - eBilling - Transmit 837 Transactions Through New Platform - Outpatient UB04– US3346</t>
-  </si>
-  <si>
-    <t>1/14/2019 Found in IB*2.0*623_T16</t>
-  </si>
-  <si>
-    <t>CIT - system is unable to id the correct Batch number if in a queue for FHIR and the switch is set to off</t>
-  </si>
-  <si>
-    <t>DE1076</t>
-  </si>
-  <si>
-    <t>1/16/2019 Found in IB*2.0*623_T16</t>
-  </si>
-  <si>
-    <t>TC3967 - CIT - eBilling Implement Release of Information – Outpatient 1500 Professional Claim_US4995 and TC3968: CIT-eBilling Implement Release of Information – Outpatient UB04 Institutional Claim</t>
-  </si>
-  <si>
-    <t>7/31/2018 Found in IB*2.0*623_T7</t>
-  </si>
-  <si>
-    <t>8/7/2018 Verified in IB*2.0*623_T8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/22/2019 Verified in IB*2.0*623_T20 </t>
-  </si>
-  <si>
-    <t>UAT defect</t>
-  </si>
-  <si>
-    <t>May 2019</t>
+    <t>Updated with Defect found in IOC testing</t>
+  </si>
+  <si>
+    <t>IOC - Claim had structure under procedure code without actual procedure code</t>
+  </si>
+  <si>
+    <t>DE1476</t>
+  </si>
+  <si>
+    <t>6/26/2019 Found in IB*2.0*623 T21</t>
+  </si>
+  <si>
+    <t>7/9/2019 Verified in IB*2.0*623 T23</t>
+  </si>
+  <si>
+    <t>IOC - Error or routine to be matched: IBCEFP</t>
+  </si>
+  <si>
+    <t>DE1483</t>
+  </si>
+  <si>
+    <t>7/1/2019 Found in IB*2.0*623 T21</t>
+  </si>
+  <si>
+    <t>IOC - lookup by external claim number when getting claims in FHIR bundled format</t>
+  </si>
+  <si>
+    <t>DE1495</t>
+  </si>
+  <si>
+    <t>IOC - Alow claims to be sent in RCB even if Test</t>
+  </si>
+  <si>
+    <t>DE1497</t>
+  </si>
+  <si>
+    <t>IOC - When FHIR retransmits live claims as test,  EOB information received for payers</t>
+  </si>
+  <si>
+    <t>DE1499</t>
   </si>
 </sst>
 </file>
@@ -1965,7 +2037,7 @@
   <dimension ref="A5:H34"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:H23"/>
+      <selection activeCell="A26" sqref="A26:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2046,7 +2118,7 @@
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
@@ -2066,7 +2138,7 @@
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="49" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="B26" s="49"/>
       <c r="C26" s="49"/>
@@ -2112,7 +2184,7 @@
   <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2148,7 +2220,7 @@
     </row>
     <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
@@ -2160,11 +2232,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="11"/>
+    <row r="5" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
@@ -2236,8 +2316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2304,7 +2384,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>25</v>
@@ -2313,19 +2393,19 @@
         <v>26</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>8</v>
@@ -2334,28 +2414,28 @@
         <v>19</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>8</v>
@@ -2364,30 +2444,30 @@
         <v>19</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="28" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J4" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="44" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>8</v>
@@ -2396,28 +2476,28 @@
         <v>19</v>
       </c>
       <c r="F5" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="28" t="s">
         <v>114</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>115</v>
       </c>
       <c r="J5" s="43"/>
     </row>
     <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>8</v>
@@ -2426,28 +2506,28 @@
         <v>19</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="I6" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>8</v>
@@ -2456,28 +2536,28 @@
         <v>19</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="I7" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" s="30"/>
     </row>
     <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>8</v>
@@ -2486,28 +2566,28 @@
         <v>19</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G8" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="I8" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J8" s="30"/>
     </row>
     <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>21</v>
@@ -2516,28 +2596,28 @@
         <v>19</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G9" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="28" t="s">
-        <v>49</v>
-      </c>
       <c r="I9" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J9" s="30"/>
     </row>
     <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>8</v>
@@ -2546,30 +2626,30 @@
         <v>19</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G10" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="28" t="s">
-        <v>53</v>
-      </c>
       <c r="I10" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>8</v>
@@ -2578,28 +2658,28 @@
         <v>19</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G11" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="I11" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J11" s="30"/>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>8</v>
@@ -2608,28 +2688,28 @@
         <v>19</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G12" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="I12" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J12" s="30"/>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>20</v>
@@ -2638,28 +2718,28 @@
         <v>19</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G13" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="I13" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J13" s="30"/>
     </row>
     <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>20</v>
@@ -2668,28 +2748,28 @@
         <v>19</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="I14" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J14" s="30"/>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>8</v>
@@ -2698,28 +2778,28 @@
         <v>19</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I15" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J15" s="30"/>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>20</v>
@@ -2728,28 +2808,28 @@
         <v>19</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G16" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="I16" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J16" s="30"/>
     </row>
     <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>8</v>
@@ -2758,28 +2838,28 @@
         <v>19</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G17" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="I17" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J17" s="30"/>
     </row>
     <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>20</v>
@@ -2788,28 +2868,28 @@
         <v>19</v>
       </c>
       <c r="F18" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="28" t="s">
         <v>87</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>88</v>
       </c>
       <c r="J18" s="30"/>
     </row>
     <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="28" t="s">
         <v>8</v>
@@ -2818,28 +2898,28 @@
         <v>19</v>
       </c>
       <c r="F19" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="28" t="s">
         <v>87</v>
-      </c>
-      <c r="G19" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" s="28" t="s">
-        <v>88</v>
       </c>
       <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="28" t="s">
         <v>21</v>
@@ -2848,28 +2928,28 @@
         <v>19</v>
       </c>
       <c r="F20" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" s="28" t="s">
         <v>98</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>99</v>
       </c>
       <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D21" s="42" t="s">
         <v>8</v>
@@ -2878,28 +2958,28 @@
         <v>19</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G21" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="I21" s="28" t="s">
         <v>103</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>104</v>
       </c>
       <c r="J21" s="30"/>
     </row>
     <row r="22" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D22" s="28" t="s">
         <v>20</v>
@@ -2908,28 +2988,28 @@
         <v>19</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G22" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H22" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="H22" s="28" t="s">
-        <v>108</v>
-      </c>
       <c r="I22" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J22" s="30"/>
     </row>
     <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D23" s="42" t="s">
         <v>8</v>
@@ -2938,114 +3018,258 @@
         <v>19</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G23" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="H23" s="28" t="s">
-        <v>108</v>
-      </c>
       <c r="I23" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J23" s="30"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
+    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>121</v>
+      </c>
       <c r="J24" s="30"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
+    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>133</v>
+      </c>
       <c r="J25" s="30"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="28"/>
+    <row r="26" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>121</v>
+      </c>
       <c r="J26" s="39"/>
       <c r="M26" s="41"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
+    <row r="27" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>133</v>
+      </c>
       <c r="J27" s="30"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="28"/>
+    <row r="28" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>133</v>
+      </c>
       <c r="J28" s="30"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
+    <row r="29" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>133</v>
+      </c>
       <c r="J29" s="30"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
+    <row r="30" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>133</v>
+      </c>
       <c r="J30" s="30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
+    <row r="31" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I31" s="28" t="s">
+        <v>133</v>
+      </c>
       <c r="J31" s="30"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>